<commit_message>
#5 Notes should be imported. Ensure zipcode format. Improvement for mailing address displaying format
</commit_message>
<xml_diff>
--- a/spec/factories/Sample Companies.xlsx
+++ b/spec/factories/Sample Companies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Company Name</t>
   </si>
@@ -155,6 +155,30 @@
   </si>
   <si>
     <t>Client, Vendor</t>
+  </si>
+  <si>
+    <t>Huge Organization</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -227,12 +251,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -240,9 +267,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,11 +623,13 @@
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,19 +640,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -631,16 +672,28 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>78701</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -651,16 +704,25 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>78702</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -671,16 +733,25 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>78703</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -691,16 +762,25 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>78704</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -711,17 +791,26 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>78705</v>
+      </c>
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -732,16 +821,25 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>78706</v>
+      </c>
+      <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -752,16 +850,25 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>78707</v>
+      </c>
+      <c r="G8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -772,16 +879,25 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>800001</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -792,16 +908,25 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10">
+        <v>800002</v>
+      </c>
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -812,16 +937,25 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11">
+        <v>800003</v>
+      </c>
+      <c r="G11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -832,21 +966,31 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <v>800004</v>
+      </c>
+      <c r="G12" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+    <row r="13" spans="1:10">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>